<commit_message>
Arranged activity places in workflow.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\IT05\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\IT06\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0FC70-9BDF-4841-8145-8AB857EB9101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5C6956-0ACF-47A1-8C31-F9A7EABD8C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -156,9 +156,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
@@ -250,13 +247,22 @@
   </si>
   <si>
     <t>Uygulma Sunucusu İşletim Sistemi</t>
+  </si>
+  <si>
+    <t>RAS IT06</t>
+  </si>
+  <si>
+    <t>DelayDuration</t>
+  </si>
+  <si>
+    <t>00:00:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -273,6 +279,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -295,11 +308,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -668,118 +683,118 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
         <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
         <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1778,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2009,18 +2024,25 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2995,6 +3017,7 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>